<commit_message>
Regenated output files after the changes made. CIFMM-2445
</commit_message>
<xml_diff>
--- a/output/SharedMedicinesList/medication-known-1.xlsx
+++ b/output/SharedMedicinesList/medication-known-1.xlsx
@@ -346,7 +346,7 @@
 </t>
   </si>
   <si>
-    <t>Medication Brand Name</t>
+    <t>Medication brand name</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1
@@ -354,7 +354,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
     <t>genericName</t>
@@ -364,7 +364,7 @@
 </t>
   </si>
   <si>
-    <t>Medication Generic Drug Name</t>
+    <t>Medication generic drug name</t>
   </si>
   <si>
     <t>strengthText</t>
@@ -374,7 +374,7 @@
 </t>
   </si>
   <si>
-    <t>Medication Strength Text</t>
+    <t>Medication strength text</t>
   </si>
   <si>
     <t>A textual representation of medication strength to support systems with limited atomic ingredient data support.</t>

</xml_diff>